<commit_message>
fix error in batch file
</commit_message>
<xml_diff>
--- a/data/2025_01_23_RepoMetaCuration.xlsx
+++ b/data/2025_01_23_RepoMetaCuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtsueng\Anaconda3\envs\nde\nde_meta_batch_converter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F3B0FD-9433-4685-B5CC-6A15035E59B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953814DC-E132-42B4-8174-DE102CBDC7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12216" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12216" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resource_base" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="502">
   <si>
     <t>name</t>
   </si>
@@ -1724,6 +1724,21 @@
   </si>
   <si>
     <t>https://www.iddo.org/wwarn/wwarn-vivax-library</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42651</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C19026</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C47824</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C17146</t>
+  </si>
+  <si>
+    <t>http://schema.org/Course</t>
   </si>
 </sst>
 </file>
@@ -5263,7 +5278,7 @@
     <col min="1" max="1" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -9375,7 +9390,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD15"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9383,7 +9398,7 @@
     <col min="1" max="1" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -9517,7 +9532,7 @@
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -9675,7 +9690,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A29" sqref="A29:XFD39"/>
     </sheetView>
   </sheetViews>
@@ -9684,7 +9699,7 @@
     <col min="1" max="1" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -10254,7 +10269,7 @@
     <col min="1" max="1" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -11132,9 +11147,9 @@
   </sheetPr>
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A94" sqref="A94:XFD124"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12054,7 +12069,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65" s="16" t="s">
         <v>58</v>
       </c>
@@ -12068,7 +12083,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A66" s="16" t="s">
         <v>58</v>
       </c>
@@ -12082,7 +12097,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A67" s="16" t="s">
         <v>58</v>
       </c>
@@ -12092,11 +12107,14 @@
       <c r="C67" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="D67" s="23" t="s">
+      <c r="D67" t="s">
+        <v>497</v>
+      </c>
+      <c r="E67" s="23" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A68" s="16" t="s">
         <v>58</v>
       </c>
@@ -12106,11 +12124,14 @@
       <c r="C68" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D68" s="23" t="s">
+      <c r="D68" t="s">
+        <v>498</v>
+      </c>
+      <c r="E68" s="23" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
         <v>58</v>
       </c>
@@ -12120,11 +12141,14 @@
       <c r="C69" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D69" s="23" t="s">
+      <c r="D69" t="s">
+        <v>499</v>
+      </c>
+      <c r="E69" s="23" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
         <v>58</v>
       </c>
@@ -12134,11 +12158,14 @@
       <c r="C70" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D70" s="10" t="s">
+      <c r="D70" t="s">
+        <v>500</v>
+      </c>
+      <c r="E70" s="10" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
         <v>65</v>
       </c>
@@ -12152,7 +12179,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
         <v>65</v>
       </c>
@@ -12166,7 +12193,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
         <v>65</v>
       </c>
@@ -12180,7 +12207,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
         <v>65</v>
       </c>
@@ -12194,7 +12221,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A75" s="16" t="s">
         <v>65</v>
       </c>
@@ -12208,7 +12235,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A76" s="16" t="s">
         <v>65</v>
       </c>
@@ -12222,7 +12249,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A77" s="16" t="s">
         <v>65</v>
       </c>
@@ -12236,7 +12263,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A78" s="16" t="s">
         <v>65</v>
       </c>
@@ -12250,7 +12277,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A79" s="16" t="s">
         <v>65</v>
       </c>
@@ -12264,7 +12291,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A80" s="16" t="s">
         <v>65</v>
       </c>
@@ -12278,7 +12305,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A81" s="16" t="s">
         <v>65</v>
       </c>
@@ -12292,7 +12319,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A82" s="16" t="s">
         <v>65</v>
       </c>
@@ -12306,7 +12333,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A83" s="16" t="s">
         <v>65</v>
       </c>
@@ -12320,7 +12347,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A84" s="16" t="s">
         <v>65</v>
       </c>
@@ -12334,7 +12361,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A85" s="16" t="s">
         <v>65</v>
       </c>
@@ -12348,7 +12375,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A86" s="16" t="s">
         <v>65</v>
       </c>
@@ -12362,7 +12389,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A87" s="16" t="s">
         <v>65</v>
       </c>
@@ -12376,7 +12403,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A88" s="16" t="s">
         <v>65</v>
       </c>
@@ -12390,7 +12417,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A89" s="16" t="s">
         <v>65</v>
       </c>
@@ -12400,11 +12427,14 @@
       <c r="C89" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="D89" s="23" t="s">
+      <c r="D89" t="s">
+        <v>497</v>
+      </c>
+      <c r="E89" s="23" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A90" s="16" t="s">
         <v>65</v>
       </c>
@@ -12414,11 +12444,14 @@
       <c r="C90" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D90" s="23" t="s">
+      <c r="D90" t="s">
+        <v>498</v>
+      </c>
+      <c r="E90" s="23" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A91" s="16" t="s">
         <v>65</v>
       </c>
@@ -12428,11 +12461,14 @@
       <c r="C91" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D91" s="23" t="s">
+      <c r="D91" t="s">
+        <v>499</v>
+      </c>
+      <c r="E91" s="23" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A92" s="16" t="s">
         <v>65</v>
       </c>
@@ -12442,11 +12478,14 @@
       <c r="C92" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="D92" s="23" t="s">
+      <c r="D92" t="s">
+        <v>501</v>
+      </c>
+      <c r="E92" s="23" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A93" s="16" t="s">
         <v>65</v>
       </c>
@@ -12456,7 +12495,10 @@
       <c r="C93" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D93" s="10" t="s">
+      <c r="D93" t="s">
+        <v>500</v>
+      </c>
+      <c r="E93" s="10" t="s">
         <v>470</v>
       </c>
     </row>
@@ -12595,11 +12637,11 @@
     <hyperlink ref="A66" r:id="rId131" xr:uid="{00000000-0004-0000-0600-000010040000}"/>
     <hyperlink ref="D66" r:id="rId132" xr:uid="{00000000-0004-0000-0600-000011040000}"/>
     <hyperlink ref="A67" r:id="rId133" xr:uid="{00000000-0004-0000-0600-000012040000}"/>
-    <hyperlink ref="D67" r:id="rId134" xr:uid="{00000000-0004-0000-0600-000013040000}"/>
+    <hyperlink ref="E67" r:id="rId134" xr:uid="{00000000-0004-0000-0600-000013040000}"/>
     <hyperlink ref="A68" r:id="rId135" xr:uid="{00000000-0004-0000-0600-000014040000}"/>
-    <hyperlink ref="D68" r:id="rId136" xr:uid="{00000000-0004-0000-0600-000015040000}"/>
+    <hyperlink ref="E68" r:id="rId136" xr:uid="{00000000-0004-0000-0600-000015040000}"/>
     <hyperlink ref="A69" r:id="rId137" xr:uid="{00000000-0004-0000-0600-000016040000}"/>
-    <hyperlink ref="D69" r:id="rId138" xr:uid="{00000000-0004-0000-0600-000017040000}"/>
+    <hyperlink ref="E69" r:id="rId138" xr:uid="{00000000-0004-0000-0600-000017040000}"/>
     <hyperlink ref="A70" r:id="rId139" xr:uid="{00000000-0004-0000-0600-000018040000}"/>
     <hyperlink ref="A71" r:id="rId140" xr:uid="{00000000-0004-0000-0600-000019040000}"/>
     <hyperlink ref="D71" r:id="rId141" xr:uid="{00000000-0004-0000-0600-00001A040000}"/>
@@ -12638,16 +12680,17 @@
     <hyperlink ref="A88" r:id="rId174" xr:uid="{00000000-0004-0000-0600-00003B040000}"/>
     <hyperlink ref="D88" r:id="rId175" xr:uid="{00000000-0004-0000-0600-00003C040000}"/>
     <hyperlink ref="A89" r:id="rId176" xr:uid="{00000000-0004-0000-0600-00003D040000}"/>
-    <hyperlink ref="D89" r:id="rId177" xr:uid="{00000000-0004-0000-0600-00003E040000}"/>
+    <hyperlink ref="E89" r:id="rId177" xr:uid="{00000000-0004-0000-0600-00003E040000}"/>
     <hyperlink ref="A90" r:id="rId178" xr:uid="{00000000-0004-0000-0600-00003F040000}"/>
-    <hyperlink ref="D90" r:id="rId179" xr:uid="{00000000-0004-0000-0600-000040040000}"/>
+    <hyperlink ref="E90" r:id="rId179" xr:uid="{00000000-0004-0000-0600-000040040000}"/>
     <hyperlink ref="A91" r:id="rId180" xr:uid="{00000000-0004-0000-0600-000041040000}"/>
-    <hyperlink ref="D91" r:id="rId181" xr:uid="{00000000-0004-0000-0600-000042040000}"/>
+    <hyperlink ref="E91" r:id="rId181" xr:uid="{00000000-0004-0000-0600-000042040000}"/>
     <hyperlink ref="A92" r:id="rId182" xr:uid="{00000000-0004-0000-0600-000043040000}"/>
-    <hyperlink ref="D92" r:id="rId183" xr:uid="{00000000-0004-0000-0600-000044040000}"/>
+    <hyperlink ref="E92" r:id="rId183" xr:uid="{00000000-0004-0000-0600-000044040000}"/>
     <hyperlink ref="A93" r:id="rId184" xr:uid="{00000000-0004-0000-0600-000045040000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId185"/>
 </worksheet>
 </file>
 
@@ -12658,14 +12701,14 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>

</xml_diff>